<commit_message>
atualização caminho relativo e driver
</commit_message>
<xml_diff>
--- a/src/test/java/br/com/rsinet/hub/bdd/testdata/TestData.xlsx
+++ b/src/test/java/br/com/rsinet/hub/bdd/testdata/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilker.nogueira\eclipse-workspace\avaliacao-automacao-tdd\src\test\java\br\com\rsinet\hub\tdd\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilker.nogueira\eclipse-workspace-automacao\avaliacao-automacao-bdd\src\test\java\br\com\rsinet\hub\bdd\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD02C6B-6FAD-4E44-B643-F3CE235C6E20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D38CE80-06CB-453F-A4CE-165D3E5ED31B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20640" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{8A0BD1D9-DBE4-467F-9B03-07923CE60D62}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" firstSheet="1" activeTab="1" xr2:uid="{8A0BD1D9-DBE4-467F-9B03-07923CE60D62}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -289,7 +289,7 @@
     <t>C(13,0) V(13,1)</t>
   </si>
   <si>
-    <t>Wilkerbn501</t>
+    <t>Wilkerbn502</t>
   </si>
 </sst>
 </file>

</xml_diff>